<commit_message>
added new module decorator in libs
</commit_message>
<xml_diff>
--- a/Бланк заказа.xlsx
+++ b/Бланк заказа.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruslan/PycharmProjects/oldcodersclub/subcategories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgi/Documents/NewEraProg/pythonProject1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD18309-EBE1-C344-96AF-2A235035BFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CEC2A8-33D4-2141-BF23-9E9893F1CACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1300" windowWidth="25320" windowHeight="19860" tabRatio="361" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="361" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Бланк Заказа" sheetId="1" r:id="rId1"/>
@@ -4445,7 +4445,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4466,9 +4466,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4506,7 +4506,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4612,7 +4612,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4792,11 +4792,11 @@
   </sheetPr>
   <dimension ref="B1:L743"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="12" ySplit="5" topLeftCell="M706" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="12" ySplit="5" topLeftCell="M6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="T1" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B712" sqref="B712"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="11.5" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>